<commit_message>
added suite xml to pom
</commit_message>
<xml_diff>
--- a/testdata/OpenEmrData.xlsx
+++ b/testdata/OpenEmrData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7380" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7380"/>
   </bookViews>
   <sheets>
     <sheet name="invalidCredentialData" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
   <si>
     <t>Password</t>
   </si>
@@ -45,25 +45,10 @@
     <t>English (Indian)</t>
   </si>
   <si>
-    <t>admin456</t>
-  </si>
-  <si>
-    <t>pass456</t>
-  </si>
-  <si>
     <t>pass123</t>
   </si>
   <si>
     <t>Username</t>
-  </si>
-  <si>
-    <t>admin789</t>
-  </si>
-  <si>
-    <t>admin888</t>
-  </si>
-  <si>
-    <t>admin555</t>
   </si>
   <si>
     <t>admin</t>
@@ -421,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,7 +422,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -454,68 +439,12 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
         <v>3</v>
       </c>
     </row>
@@ -528,7 +457,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
@@ -543,7 +472,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -552,16 +481,16 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="H1" t="s">
         <v>2</v>
@@ -569,54 +498,54 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="H2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" t="s">
         <v>20</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>